<commit_message>
fix installation problem, lot of bug fix
</commit_message>
<xml_diff>
--- a/examples/sample_annotation_file.xlsx
+++ b/examples/sample_annotation_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\kyao\dev\t2wml-projects\projects\aid\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minazuki/Desktop/studies/master/2018Summer/dsbox_2019/t2wml-projects/projects/aid/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D1FEB8-8BCE-4BFC-ABE1-78FBDECAAED8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CD91EE-0CF3-8D4E-9637-B979DC526633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29890" yWindow="-1630" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="3560" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - aid worker security_i" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="174">
   <si>
     <t>dataset</t>
   </si>
@@ -565,16 +565,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="7">
@@ -615,7 +619,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -655,17 +659,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -843,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -871,79 +864,79 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -958,27 +951,21 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1196,52 +1183,52 @@
   </sheetPr>
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="AD8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="AN2" sqref="AN2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.703125" customWidth="1"/>
-    <col min="2" max="2" width="32.29296875" customWidth="1"/>
-    <col min="3" max="3" width="7.5859375" customWidth="1"/>
-    <col min="4" max="4" width="9.29296875" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="10.5859375" customWidth="1"/>
-    <col min="7" max="8" width="11.87890625" customWidth="1"/>
-    <col min="9" max="9" width="40.87890625" customWidth="1"/>
-    <col min="10" max="11" width="10.41015625" customWidth="1"/>
-    <col min="12" max="12" width="12.41015625" customWidth="1"/>
-    <col min="13" max="13" width="5.703125" customWidth="1"/>
-    <col min="14" max="14" width="5.29296875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="40.83203125" customWidth="1"/>
+    <col min="10" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
-    <col min="16" max="16" width="13.703125" customWidth="1"/>
-    <col min="17" max="17" width="16.87890625" customWidth="1"/>
-    <col min="18" max="18" width="17.87890625" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" customWidth="1"/>
+    <col min="18" max="18" width="17.83203125" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="17.1171875" customWidth="1"/>
-    <col min="21" max="21" width="20.1171875" customWidth="1"/>
-    <col min="22" max="22" width="21.29296875" customWidth="1"/>
-    <col min="23" max="23" width="16.703125" customWidth="1"/>
+    <col min="20" max="20" width="17.1640625" customWidth="1"/>
+    <col min="21" max="21" width="20.1640625" customWidth="1"/>
+    <col min="22" max="22" width="21.33203125" customWidth="1"/>
+    <col min="23" max="23" width="16.6640625" customWidth="1"/>
     <col min="24" max="24" width="10" customWidth="1"/>
-    <col min="25" max="25" width="13.1171875" customWidth="1"/>
-    <col min="26" max="26" width="14.1171875" customWidth="1"/>
-    <col min="27" max="27" width="12.29296875" customWidth="1"/>
-    <col min="28" max="28" width="11.703125" customWidth="1"/>
-    <col min="29" max="29" width="13.41015625" customWidth="1"/>
-    <col min="30" max="30" width="15.29296875" customWidth="1"/>
-    <col min="31" max="31" width="14.29296875" customWidth="1"/>
-    <col min="32" max="32" width="14.703125" customWidth="1"/>
-    <col min="33" max="33" width="12.41015625" customWidth="1"/>
-    <col min="34" max="35" width="10.29296875" customWidth="1"/>
-    <col min="36" max="36" width="19.87890625" customWidth="1"/>
-    <col min="37" max="37" width="22.41015625" customWidth="1"/>
-    <col min="38" max="38" width="51.703125" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" customWidth="1"/>
+    <col min="26" max="26" width="14.1640625" customWidth="1"/>
+    <col min="27" max="27" width="12.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.6640625" customWidth="1"/>
+    <col min="29" max="29" width="13.33203125" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" customWidth="1"/>
+    <col min="31" max="31" width="14.33203125" customWidth="1"/>
+    <col min="32" max="32" width="14.6640625" customWidth="1"/>
+    <col min="33" max="33" width="12.33203125" customWidth="1"/>
+    <col min="34" max="35" width="10.33203125" customWidth="1"/>
+    <col min="36" max="36" width="19.83203125" customWidth="1"/>
+    <col min="37" max="37" width="22.33203125" customWidth="1"/>
+    <col min="38" max="38" width="51.6640625" customWidth="1"/>
     <col min="39" max="39" width="8" customWidth="1"/>
-    <col min="40" max="40" width="9.87890625" customWidth="1"/>
+    <col min="40" max="40" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="19.5" customHeight="1">
@@ -1296,56 +1283,120 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="42" t="s">
+      <c r="D2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="43" t="s">
+      <c r="G2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="40"/>
-      <c r="AE2" s="38" t="s">
+      <c r="K2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="40"/>
-      <c r="AH2" s="42" t="s">
+      <c r="AF2" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG2" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="AI2" s="40"/>
-      <c r="AJ2" s="38" t="s">
+      <c r="AI2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="40"/>
+      <c r="AK2" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL2" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM2" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN2" s="41" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:40" ht="19.5" customHeight="1">
       <c r="A3" s="3" t="s">
@@ -46042,14 +46093,7 @@
       <c r="AN1000" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="AJ2:AN2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
@@ -46068,7 +46112,7 @@
           <x14:formula1>
             <xm:f>role!$A$1:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:C2 F2 J2 AE2 AH2 AJ2</xm:sqref>
+          <xm:sqref>B2:AN2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -46085,39 +46129,40 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -46131,74 +46176,75 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="15" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" ht="15" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" ht="15" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" ht="15" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>171</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>